<commit_message>
Updating all workbooks for findings.
</commit_message>
<xml_diff>
--- a/assets/findings/2024-02-03-findings.xlsx
+++ b/assets/findings/2024-02-03-findings.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U18"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,24 +432,25 @@
     <col width="4.8" customWidth="1" min="1" max="1"/>
     <col width="32.4" customWidth="1" min="2" max="2"/>
     <col width="48" customWidth="1" min="3" max="3"/>
-    <col width="20.4" customWidth="1" min="4" max="4"/>
-    <col width="21.6" customWidth="1" min="5" max="5"/>
-    <col width="9.6" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="58.8" customWidth="1" min="8" max="8"/>
-    <col width="20.4" customWidth="1" min="9" max="9"/>
-    <col width="13.2" customWidth="1" min="10" max="10"/>
-    <col width="12" customWidth="1" min="11" max="11"/>
-    <col width="26.4" customWidth="1" min="12" max="12"/>
-    <col width="24" customWidth="1" min="13" max="13"/>
-    <col width="25.2" customWidth="1" min="14" max="14"/>
-    <col width="21.6" customWidth="1" min="15" max="15"/>
-    <col width="26.4" customWidth="1" min="16" max="16"/>
-    <col width="32.4" customWidth="1" min="17" max="17"/>
-    <col width="22.8" customWidth="1" min="18" max="18"/>
-    <col width="25.2" customWidth="1" min="19" max="19"/>
-    <col width="22.8" customWidth="1" min="20" max="20"/>
-    <col width="32.4" customWidth="1" min="21" max="21"/>
+    <col width="16.8" customWidth="1" min="4" max="4"/>
+    <col width="20.4" customWidth="1" min="5" max="5"/>
+    <col width="21.6" customWidth="1" min="6" max="6"/>
+    <col width="9.6" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="58.8" customWidth="1" min="9" max="9"/>
+    <col width="20.4" customWidth="1" min="10" max="10"/>
+    <col width="13.2" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="26.4" customWidth="1" min="13" max="13"/>
+    <col width="24" customWidth="1" min="14" max="14"/>
+    <col width="25.2" customWidth="1" min="15" max="15"/>
+    <col width="21.6" customWidth="1" min="16" max="16"/>
+    <col width="26.4" customWidth="1" min="17" max="17"/>
+    <col width="32.4" customWidth="1" min="18" max="18"/>
+    <col width="22.8" customWidth="1" min="19" max="19"/>
+    <col width="25.2" customWidth="1" min="20" max="20"/>
+    <col width="22.8" customWidth="1" min="21" max="21"/>
+    <col width="32.4" customWidth="1" min="22" max="22"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -470,90 +471,95 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>auditee_uei</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>award_reference</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>reference_number</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>aln</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>cog_over</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>federal_program_name</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>amount_expended</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>is_direct</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>is_major</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>is_passthrough_award</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>passthrough_amount</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>is_modified_opinion</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>is_other_matters</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>is_material_weakness</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>is_significant_deficiency</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>is_other_findings</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>is_questioned_costs</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>is_repeat_finding</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>prior_finding_ref_numbers</t>
         </is>
@@ -575,32 +581,34 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>AWARD-0001</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>2023-001</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>84.027</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>SPECIAL EDUCATION_GRANTS TO STATES</t>
         </is>
       </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
       <c r="J2" t="inlineStr">
         <is>
           <t>NO</t>
@@ -616,10 +624,8 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="M2" t="b">
+        <v>0</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -636,22 +642,25 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R2" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="T2" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S2" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="U2" t="b">
+        <v>1</v>
+      </c>
+      <c r="V2" t="inlineStr">
         <is>
           <t>2022-002</t>
         </is>
@@ -673,32 +682,34 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>AWARD-0002</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>84.425</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>EDUCATION STABILIZATION FUND</t>
         </is>
       </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
       <c r="J3" t="inlineStr">
         <is>
           <t>NO</t>
@@ -714,10 +725,8 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="M3" t="b">
+        <v>0</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -734,14 +743,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R3" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S3" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
@@ -749,7 +758,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="U3" t="b">
+        <v>0</v>
+      </c>
+      <c r="V3" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -771,32 +783,34 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>AWARD-0003</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>84.425</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>EDUCATION STABILIZATION FUND</t>
         </is>
       </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
       <c r="J4" t="inlineStr">
         <is>
           <t>NO</t>
@@ -812,10 +826,8 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="M4" t="b">
+        <v>0</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -832,14 +844,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R4" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S4" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
@@ -847,7 +859,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U4" t="inlineStr">
+      <c r="U4" t="b">
+        <v>0</v>
+      </c>
+      <c r="V4" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -869,37 +884,37 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>AWARD-0012</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>84.173</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>SPECIAL EDUCATION_PRESCHOOL GRANTS</t>
         </is>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>662</v>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
       <c r="K5" t="inlineStr">
         <is>
           <t>NO</t>
@@ -910,10 +925,8 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="M5" t="b">
+        <v>0</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -930,14 +943,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R5" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S5" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
@@ -945,7 +958,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U5" t="inlineStr">
+      <c r="U5" t="b">
+        <v>0</v>
+      </c>
+      <c r="V5" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -967,37 +983,37 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>AWARD-0014</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>84.010</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>TITLE I GRANTS TO LOCAL EDUCATIONAL AGENCIES</t>
         </is>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>622737</v>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
       <c r="K6" t="inlineStr">
         <is>
           <t>NO</t>
@@ -1008,10 +1024,8 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="M6" t="b">
+        <v>0</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -1028,14 +1042,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R6" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S6" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
@@ -1043,7 +1057,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U6" t="inlineStr">
+      <c r="U6" t="b">
+        <v>0</v>
+      </c>
+      <c r="V6" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1065,37 +1082,37 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>AWARD-0016</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>84.367</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>IMPROVING TEACHER QUALITY STATE GRANTS</t>
         </is>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>56149</v>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>NO</t>
@@ -1106,10 +1123,8 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="M7" t="b">
+        <v>0</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -1126,14 +1141,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R7" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S7" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
@@ -1141,7 +1156,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U7" t="inlineStr">
+      <c r="U7" t="b">
+        <v>0</v>
+      </c>
+      <c r="V7" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1163,37 +1181,37 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>AWARD-0018</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>84.424</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>STUDENT SUPPORT AND ACADEMIC ENRICHMENT PROGRAM</t>
         </is>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>49198</v>
       </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
       <c r="K8" t="inlineStr">
         <is>
           <t>NO</t>
@@ -1204,10 +1222,8 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="M8" t="b">
+        <v>0</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1224,14 +1240,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R8" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S8" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
@@ -1239,7 +1255,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U8" t="inlineStr">
+      <c r="U8" t="b">
+        <v>0</v>
+      </c>
+      <c r="V8" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1261,37 +1280,37 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>AWARD-0020</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>84.365</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>ENGLISH LANGUAGE ACQUISITION STATE GRANTS</t>
         </is>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>14828</v>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
       <c r="K9" t="inlineStr">
         <is>
           <t>NO</t>
@@ -1302,10 +1321,8 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="M9" t="b">
+        <v>0</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1322,14 +1339,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R9" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S9" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
@@ -1337,7 +1354,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U9" t="inlineStr">
+      <c r="U9" t="b">
+        <v>0</v>
+      </c>
+      <c r="V9" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1359,51 +1379,49 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
           <t>AWARD-0021</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>2023-005</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>84.425</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>EDUCATION STABILIZATION FUND</t>
         </is>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>258507</v>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K10" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="L10" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M10" t="b">
+        <v>0</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1420,9 +1438,9 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R10" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
       <c r="S10" s="1" t="inlineStr">
@@ -1430,12 +1448,15 @@
           <t>YES</t>
         </is>
       </c>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="U10" t="inlineStr">
+      <c r="T10" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="U10" t="b">
+        <v>0</v>
+      </c>
+      <c r="V10" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1457,51 +1478,49 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>AWARD-0023</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>84.425</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>EDUCATION STABILIZATION FUND</t>
         </is>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>753845</v>
       </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K11" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="L11" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M11" t="b">
+        <v>0</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1518,14 +1537,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R11" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S11" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
@@ -1533,7 +1552,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U11" t="inlineStr">
+      <c r="U11" t="b">
+        <v>0</v>
+      </c>
+      <c r="V11" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1555,51 +1577,49 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>AWARD-0024</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>84.425</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>EDUCATION STABILIZATION FUND</t>
         </is>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>3107</v>
       </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K12" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="L12" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M12" t="b">
+        <v>0</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1616,14 +1636,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R12" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S12" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
@@ -1631,7 +1651,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U12" t="inlineStr">
+      <c r="U12" t="b">
+        <v>0</v>
+      </c>
+      <c r="V12" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1653,51 +1676,49 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
           <t>AWARD-0025</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>2023-001</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>84.425</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>EDUCATION STABILIZATION FUND</t>
         </is>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>215</v>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K13" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="L13" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M13" t="b">
+        <v>0</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1714,22 +1735,25 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R13" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="T13" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="U13" t="inlineStr">
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S13" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="U13" t="b">
+        <v>1</v>
+      </c>
+      <c r="V13" t="inlineStr">
         <is>
           <t>2022-002</t>
         </is>
@@ -1751,51 +1775,49 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>AWARD-0026</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>2023-003</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>84.425</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>EDUCATION STABILIZATION FUND</t>
         </is>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
         <v>79485</v>
       </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K14" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="L14" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M14" t="b">
+        <v>0</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1812,9 +1834,9 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R14" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
       <c r="S14" s="1" t="inlineStr">
@@ -1822,12 +1844,15 @@
           <t>YES</t>
         </is>
       </c>
-      <c r="T14" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="U14" t="inlineStr">
+      <c r="T14" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="U14" t="b">
+        <v>0</v>
+      </c>
+      <c r="V14" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1849,51 +1874,49 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
           <t>AWARD-0028</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>84.425</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>EDUCATION STABILIZATION FUND</t>
         </is>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>240537</v>
       </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K15" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="L15" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M15" t="b">
+        <v>0</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1910,14 +1933,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R15" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S15" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T15" t="inlineStr">
@@ -1925,7 +1948,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U15" t="inlineStr">
+      <c r="U15" t="b">
+        <v>0</v>
+      </c>
+      <c r="V15" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1947,51 +1973,49 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
           <t>AWARD-0028</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>2023-004</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>84.425</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>EDUCATION STABILIZATION FUND</t>
         </is>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>240537</v>
       </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K16" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="L16" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M16" t="b">
+        <v>0</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -2008,9 +2032,9 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R16" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
       <c r="S16" s="1" t="inlineStr">
@@ -2018,12 +2042,15 @@
           <t>YES</t>
         </is>
       </c>
-      <c r="T16" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="U16" t="inlineStr">
+      <c r="T16" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="U16" t="b">
+        <v>0</v>
+      </c>
+      <c r="V16" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2045,32 +2072,34 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
           <t>AWARD-0031</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>84.425</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>EDUCATION STABILIZATION FUND</t>
         </is>
       </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
       <c r="J17" t="inlineStr">
         <is>
           <t>NO</t>
@@ -2086,10 +2115,8 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="M17" t="b">
+        <v>0</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -2106,14 +2133,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R17" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S17" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T17" t="inlineStr">
@@ -2121,7 +2148,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U17" t="inlineStr">
+      <c r="U17" t="b">
+        <v>0</v>
+      </c>
+      <c r="V17" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2143,32 +2173,34 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>AWARD-0032</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>84.027</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>SPECIAL EDUCATION_GRANTS TO STATES</t>
         </is>
       </c>
-      <c r="I18" t="n">
-        <v>0</v>
-      </c>
       <c r="J18" t="inlineStr">
         <is>
           <t>NO</t>
@@ -2184,10 +2216,8 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="M18" t="b">
+        <v>0</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -2204,14 +2234,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R18" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S18" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T18" t="inlineStr">
@@ -2219,7 +2249,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U18" t="inlineStr">
+      <c r="U18" t="b">
+        <v>0</v>
+      </c>
+      <c r="V18" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2272,7 +2305,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U18"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2283,24 +2316,25 @@
     <col width="4.8" customWidth="1" min="1" max="1"/>
     <col width="32.4" customWidth="1" min="2" max="2"/>
     <col width="48" customWidth="1" min="3" max="3"/>
-    <col width="20.4" customWidth="1" min="4" max="4"/>
-    <col width="21.6" customWidth="1" min="5" max="5"/>
-    <col width="9.6" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="58.8" customWidth="1" min="8" max="8"/>
-    <col width="20.4" customWidth="1" min="9" max="9"/>
-    <col width="13.2" customWidth="1" min="10" max="10"/>
-    <col width="12" customWidth="1" min="11" max="11"/>
-    <col width="26.4" customWidth="1" min="12" max="12"/>
-    <col width="24" customWidth="1" min="13" max="13"/>
-    <col width="25.2" customWidth="1" min="14" max="14"/>
-    <col width="21.6" customWidth="1" min="15" max="15"/>
-    <col width="26.4" customWidth="1" min="16" max="16"/>
-    <col width="32.4" customWidth="1" min="17" max="17"/>
-    <col width="22.8" customWidth="1" min="18" max="18"/>
-    <col width="25.2" customWidth="1" min="19" max="19"/>
-    <col width="22.8" customWidth="1" min="20" max="20"/>
-    <col width="32.4" customWidth="1" min="21" max="21"/>
+    <col width="16.8" customWidth="1" min="4" max="4"/>
+    <col width="20.4" customWidth="1" min="5" max="5"/>
+    <col width="21.6" customWidth="1" min="6" max="6"/>
+    <col width="9.6" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="58.8" customWidth="1" min="9" max="9"/>
+    <col width="20.4" customWidth="1" min="10" max="10"/>
+    <col width="13.2" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="26.4" customWidth="1" min="13" max="13"/>
+    <col width="24" customWidth="1" min="14" max="14"/>
+    <col width="25.2" customWidth="1" min="15" max="15"/>
+    <col width="21.6" customWidth="1" min="16" max="16"/>
+    <col width="26.4" customWidth="1" min="17" max="17"/>
+    <col width="32.4" customWidth="1" min="18" max="18"/>
+    <col width="22.8" customWidth="1" min="19" max="19"/>
+    <col width="25.2" customWidth="1" min="20" max="20"/>
+    <col width="22.8" customWidth="1" min="21" max="21"/>
+    <col width="32.4" customWidth="1" min="22" max="22"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2321,90 +2355,95 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>auditee_uei</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>award_reference</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>reference_number</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>aln</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>cog_over</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>federal_program_name</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>amount_expended</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>is_direct</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>is_major</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>is_passthrough_award</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>passthrough_amount</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>is_modified_opinion</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>is_other_matters</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>is_material_weakness</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>is_significant_deficiency</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>is_other_findings</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>is_questioned_costs</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>is_repeat_finding</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>prior_finding_ref_numbers</t>
         </is>
@@ -2426,32 +2465,34 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>AWARD-0001</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>2023-001</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>84.027</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>SPECIAL EDUCATION_GRANTS TO STATES</t>
         </is>
       </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
       <c r="J2" t="inlineStr">
         <is>
           <t>NO</t>
@@ -2467,10 +2508,8 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="M2" t="b">
+        <v>0</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -2487,22 +2526,25 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R2" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="T2" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S2" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="U2" t="b">
+        <v>1</v>
+      </c>
+      <c r="V2" t="inlineStr">
         <is>
           <t>2022-002</t>
         </is>
@@ -2524,32 +2566,34 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>AWARD-0002</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>84.425</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>EDUCATION STABILIZATION FUND</t>
         </is>
       </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
       <c r="J3" t="inlineStr">
         <is>
           <t>NO</t>
@@ -2565,10 +2609,8 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="M3" t="b">
+        <v>0</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -2585,14 +2627,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R3" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S3" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
@@ -2600,7 +2642,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="U3" t="b">
+        <v>0</v>
+      </c>
+      <c r="V3" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2622,32 +2667,34 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>AWARD-0003</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>84.425</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>EDUCATION STABILIZATION FUND</t>
         </is>
       </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
       <c r="J4" t="inlineStr">
         <is>
           <t>NO</t>
@@ -2663,10 +2710,8 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="M4" t="b">
+        <v>0</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -2683,14 +2728,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R4" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S4" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
@@ -2698,7 +2743,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U4" t="inlineStr">
+      <c r="U4" t="b">
+        <v>0</v>
+      </c>
+      <c r="V4" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2720,37 +2768,37 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>AWARD-0012</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>84.173</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>SPECIAL EDUCATION_PRESCHOOL GRANTS</t>
         </is>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>662</v>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
       <c r="K5" t="inlineStr">
         <is>
           <t>NO</t>
@@ -2761,10 +2809,8 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="M5" t="b">
+        <v>0</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -2781,14 +2827,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R5" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S5" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
@@ -2796,7 +2842,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U5" t="inlineStr">
+      <c r="U5" t="b">
+        <v>0</v>
+      </c>
+      <c r="V5" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2818,37 +2867,37 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>AWARD-0014</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>84.010</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>TITLE I GRANTS TO LOCAL EDUCATIONAL AGENCIES</t>
         </is>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>622737</v>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
       <c r="K6" t="inlineStr">
         <is>
           <t>NO</t>
@@ -2859,10 +2908,8 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="M6" t="b">
+        <v>0</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -2879,14 +2926,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R6" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S6" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
@@ -2894,7 +2941,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U6" t="inlineStr">
+      <c r="U6" t="b">
+        <v>0</v>
+      </c>
+      <c r="V6" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2916,37 +2966,37 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>AWARD-0016</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>84.367</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>IMPROVING TEACHER QUALITY STATE GRANTS</t>
         </is>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>56149</v>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>NO</t>
@@ -2957,10 +3007,8 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="M7" t="b">
+        <v>0</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -2977,14 +3025,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R7" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S7" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
@@ -2992,7 +3040,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U7" t="inlineStr">
+      <c r="U7" t="b">
+        <v>0</v>
+      </c>
+      <c r="V7" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3014,37 +3065,37 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>AWARD-0018</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>84.424</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>STUDENT SUPPORT AND ACADEMIC ENRICHMENT PROGRAM</t>
         </is>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>49198</v>
       </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
       <c r="K8" t="inlineStr">
         <is>
           <t>NO</t>
@@ -3055,10 +3106,8 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="M8" t="b">
+        <v>0</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -3075,14 +3124,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R8" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S8" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
@@ -3090,7 +3139,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U8" t="inlineStr">
+      <c r="U8" t="b">
+        <v>0</v>
+      </c>
+      <c r="V8" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3112,37 +3164,37 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>AWARD-0020</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>84.365</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>ENGLISH LANGUAGE ACQUISITION STATE GRANTS</t>
         </is>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>14828</v>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
       <c r="K9" t="inlineStr">
         <is>
           <t>NO</t>
@@ -3153,10 +3205,8 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="M9" t="b">
+        <v>0</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -3173,14 +3223,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R9" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S9" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
@@ -3188,7 +3238,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U9" t="inlineStr">
+      <c r="U9" t="b">
+        <v>0</v>
+      </c>
+      <c r="V9" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3210,51 +3263,49 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
           <t>AWARD-0021</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>2023-005</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>84.425</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>EDUCATION STABILIZATION FUND</t>
         </is>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>258507</v>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K10" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="L10" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M10" t="b">
+        <v>0</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -3271,9 +3322,9 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R10" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
       <c r="S10" s="1" t="inlineStr">
@@ -3281,12 +3332,15 @@
           <t>YES</t>
         </is>
       </c>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="U10" t="inlineStr">
+      <c r="T10" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="U10" t="b">
+        <v>0</v>
+      </c>
+      <c r="V10" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3308,51 +3362,49 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>AWARD-0023</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>84.425</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>EDUCATION STABILIZATION FUND</t>
         </is>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>753845</v>
       </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K11" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="L11" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M11" t="b">
+        <v>0</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -3369,14 +3421,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R11" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S11" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
@@ -3384,7 +3436,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U11" t="inlineStr">
+      <c r="U11" t="b">
+        <v>0</v>
+      </c>
+      <c r="V11" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3406,51 +3461,49 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>AWARD-0024</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>84.425</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>EDUCATION STABILIZATION FUND</t>
         </is>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>3107</v>
       </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K12" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="L12" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M12" t="b">
+        <v>0</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -3467,14 +3520,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R12" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S12" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
@@ -3482,7 +3535,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U12" t="inlineStr">
+      <c r="U12" t="b">
+        <v>0</v>
+      </c>
+      <c r="V12" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3504,51 +3560,49 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
           <t>AWARD-0025</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>2023-001</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>84.425</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>EDUCATION STABILIZATION FUND</t>
         </is>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>215</v>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K13" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="L13" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M13" t="b">
+        <v>0</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -3565,22 +3619,25 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R13" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="T13" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="U13" t="inlineStr">
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S13" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="U13" t="b">
+        <v>1</v>
+      </c>
+      <c r="V13" t="inlineStr">
         <is>
           <t>2022-002</t>
         </is>
@@ -3602,51 +3659,49 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>AWARD-0026</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>2023-003</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>84.425</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>EDUCATION STABILIZATION FUND</t>
         </is>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
         <v>79485</v>
       </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K14" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="L14" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M14" t="b">
+        <v>0</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -3663,9 +3718,9 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R14" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
       <c r="S14" s="1" t="inlineStr">
@@ -3673,12 +3728,15 @@
           <t>YES</t>
         </is>
       </c>
-      <c r="T14" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="U14" t="inlineStr">
+      <c r="T14" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="U14" t="b">
+        <v>0</v>
+      </c>
+      <c r="V14" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3700,51 +3758,49 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
           <t>AWARD-0028</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>84.425</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>EDUCATION STABILIZATION FUND</t>
         </is>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>240537</v>
       </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K15" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="L15" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M15" t="b">
+        <v>0</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -3761,14 +3817,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R15" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S15" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T15" t="inlineStr">
@@ -3776,7 +3832,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U15" t="inlineStr">
+      <c r="U15" t="b">
+        <v>0</v>
+      </c>
+      <c r="V15" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3798,51 +3857,49 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
           <t>AWARD-0028</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>2023-004</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>84.425</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>EDUCATION STABILIZATION FUND</t>
         </is>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>240537</v>
       </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K16" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="L16" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M16" t="b">
+        <v>0</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -3859,9 +3916,9 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R16" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
       <c r="S16" s="1" t="inlineStr">
@@ -3869,12 +3926,15 @@
           <t>YES</t>
         </is>
       </c>
-      <c r="T16" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="U16" t="inlineStr">
+      <c r="T16" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="U16" t="b">
+        <v>0</v>
+      </c>
+      <c r="V16" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3896,32 +3956,34 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
           <t>AWARD-0031</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>84.425</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>EDUCATION STABILIZATION FUND</t>
         </is>
       </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
       <c r="J17" t="inlineStr">
         <is>
           <t>NO</t>
@@ -3937,10 +3999,8 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="M17" t="b">
+        <v>0</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -3957,14 +4017,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R17" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S17" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T17" t="inlineStr">
@@ -3972,7 +4032,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U17" t="inlineStr">
+      <c r="U17" t="b">
+        <v>0</v>
+      </c>
+      <c r="V17" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3994,32 +4057,34 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>XLGTNB44S8N5</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>AWARD-0032</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>2023-002</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>84.027</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>OVER-84</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>SPECIAL EDUCATION_GRANTS TO STATES</t>
         </is>
       </c>
-      <c r="I18" t="n">
-        <v>0</v>
-      </c>
       <c r="J18" t="inlineStr">
         <is>
           <t>NO</t>
@@ -4035,10 +4100,8 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
+      <c r="M18" t="b">
+        <v>0</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -4055,14 +4118,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R18" s="1" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S18" s="1" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="T18" t="inlineStr">
@@ -4070,7 +4133,10 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="U18" t="inlineStr">
+      <c r="U18" t="b">
+        <v>0</v>
+      </c>
+      <c r="V18" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>

</xml_diff>